<commit_message>
COE-5098 - Changed Sharepoint folders structure.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\irina.capatina\Documents\UiPath\COE4980_AuditRobotAP\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54216909-B191-45D6-8F29-2FF726F2C1C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D982D8F-9CE3-4747-AA2F-573DD015011A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="172">
   <si>
     <t>Name</t>
   </si>
@@ -394,9 +394,6 @@
     <t>SharepointCreateFolderURL</t>
   </si>
   <si>
-    <t>ShraepointUploadFolderURL</t>
-  </si>
-  <si>
     <t>ConcurLoginURL</t>
   </si>
   <si>
@@ -521,6 +518,30 @@
   </si>
   <si>
     <t>COE4980_NSJournalSavedSeachID</t>
+  </si>
+  <si>
+    <t>TimestampFolderDateFormat</t>
+  </si>
+  <si>
+    <t>yyyy-MM-dd_HH-mm</t>
+  </si>
+  <si>
+    <t>&lt;timestamp&gt;</t>
+  </si>
+  <si>
+    <t>Will be overwritten in CleanupAndPrep</t>
+  </si>
+  <si>
+    <t>RunFolderName</t>
+  </si>
+  <si>
+    <t>RunFolderPath</t>
+  </si>
+  <si>
+    <t>SupportDocuments\RunFolderName</t>
+  </si>
+  <si>
+    <t>SharepointUploadFolderURL</t>
   </si>
 </sst>
 </file>
@@ -1193,17 +1214,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O1005"/>
+  <dimension ref="A1:O1008"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="A41" sqref="A41:XFD41"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="68" customWidth="1"/>
     <col min="2" max="2" width="70.140625" customWidth="1"/>
-    <col min="3" max="3" width="169.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="88.85546875" customWidth="1"/>
     <col min="4" max="15" width="8.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1235,7 +1256,7 @@
         <v>104</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="1"/>
@@ -1271,19 +1292,19 @@
     </row>
     <row r="5" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="B5" s="22" t="s">
         <v>150</v>
-      </c>
-      <c r="B5" s="22" t="s">
-        <v>151</v>
       </c>
       <c r="C5" s="6"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="B6" s="22" t="s">
         <v>154</v>
-      </c>
-      <c r="B6" s="22" t="s">
-        <v>155</v>
       </c>
       <c r="C6" s="6"/>
     </row>
@@ -1406,18 +1427,18 @@
     </row>
     <row r="21" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1426,18 +1447,18 @@
     </row>
     <row r="24" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1446,39 +1467,39 @@
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="B28" s="19" t="s">
         <v>141</v>
-      </c>
-      <c r="B28" s="19" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B31" s="19" t="s">
         <v>73</v>
@@ -1488,7 +1509,7 @@
       <c r="A32" s="19"/>
       <c r="B32" s="19"/>
     </row>
-    <row r="33" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>110</v>
       </c>
@@ -1496,7 +1517,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>112</v>
       </c>
@@ -1504,7 +1525,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="18" t="s">
         <v>114</v>
       </c>
@@ -1512,73 +1533,100 @@
         <v>113</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="B37" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
+      <c r="B38" s="19" t="s">
         <v>129</v>
       </c>
-      <c r="B38" s="19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="19"/>
       <c r="B39" s="19"/>
     </row>
-    <row r="40" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="B40" s="19" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="19"/>
-      <c r="B41" s="19"/>
-    </row>
-    <row r="42" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="19" t="s">
+        <v>164</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C42" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="19" t="s">
+        <v>169</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C43" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+      <c r="B44" s="19"/>
+    </row>
+    <row r="45" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="19" t="s">
+        <v>155</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="19" t="s">
         <v>156</v>
       </c>
-      <c r="B42" s="19" t="s">
+      <c r="B46" s="19" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="B43" s="19" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+    <row r="47" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="B47" s="19" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="19" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+    </row>
+    <row r="48" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="19" t="s">
         <v>161</v>
       </c>
-      <c r="B45" s="19" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="1:2" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
     <row r="49" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2536,6 +2584,9 @@
     <row r="1003" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1004" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1005" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1006" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1007" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1008" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4892,7 +4943,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4962,7 +5013,7 @@
     </row>
     <row r="5" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19" t="s">
-        <v>122</v>
+        <v>171</v>
       </c>
       <c r="B5" s="19" t="s">
         <v>118</v>
@@ -4970,26 +5021,26 @@
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="19" t="s">
         <v>163</v>
-      </c>
-      <c r="B8" s="19" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>